<commit_message>
Fix whiteList and blackList
</commit_message>
<xml_diff>
--- a/vulsList_20160225.xlsx
+++ b/vulsList_20160225.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="whiteList" sheetId="1" r:id="rId1"/>
-    <s:sheet name="blackList" sheetId="2" r:id="rId2"/>
-    <s:sheet name="vulsHistory" sheetId="3" r:id="rId3"/>
-    <s:sheet name="vuls" sheetId="4" r:id="rId4"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="570" yWindow="480" windowWidth="18000" windowHeight="7860"/>
+  </bookViews>
+  <sheets>
+    <sheet name="whiteList" sheetId="1" r:id="rId1"/>
+    <sheet name="blackList" sheetId="2" r:id="rId2"/>
+    <sheet name="vulsHistory" sheetId="3" r:id="rId3"/>
+    <sheet name="vuls" sheetId="4" r:id="rId4"/>
+  </sheets>
+  <calcPr calcId="125725"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="423">
   <si>
     <t>tech keywords</t>
   </si>
@@ -1207,108 +1207,124 @@
     <t>CVE-2016-0975</t>
   </si>
   <si>
+    <t>http://www.nsfocus.net/vulndb/32520</t>
+  </si>
+  <si>
+    <t>CVE-2016-0773</t>
+  </si>
+  <si>
+    <t>PostgreSQL权限提升漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32519</t>
+  </si>
+  <si>
+    <t>CVE-2016-0766</t>
+  </si>
+  <si>
+    <t>Microsoft .NET Framework栈缓冲区溢出漏洞(MS16-019)</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32491</t>
+  </si>
+  <si>
+    <t>CVE-2016-0033</t>
+  </si>
+  <si>
+    <t>Microsoft .NET Framework信息泄露漏洞(MS16-019)</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32490</t>
+  </si>
+  <si>
+    <t>CVE-2016-0047</t>
+  </si>
+  <si>
+    <t>Microsoft Windows PDF Library缓冲区溢出漏洞(MS16-012)</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32489</t>
+  </si>
+  <si>
+    <t>CVE-2016-0058</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Reader任意代码执行漏洞(MS16-012)</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32488</t>
+  </si>
+  <si>
+    <t>CVE-2016-0046</t>
+  </si>
+  <si>
+    <t>Microsoft Windows Journal内存破坏漏洞(MS16-013)</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32487</t>
+  </si>
+  <si>
+    <t>glibc getaddrinfo栈缓冲区溢出漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/32486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nginx </t>
+  </si>
+  <si>
+    <t>ruby</t>
+  </si>
+  <si>
+    <t>photoshop</t>
+  </si>
+  <si>
+    <t>netscaler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>PostgreSQL拒绝服务漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32520</t>
-  </si>
-  <si>
-    <t>CVE-2016-0773</t>
-  </si>
-  <si>
-    <t>PostgreSQL权限提升漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32519</t>
-  </si>
-  <si>
-    <t>CVE-2016-0766</t>
-  </si>
-  <si>
-    <t>Microsoft .NET Framework栈缓冲区溢出漏洞(MS16-019)</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32491</t>
-  </si>
-  <si>
-    <t>CVE-2016-0033</t>
-  </si>
-  <si>
-    <t>Microsoft .NET Framework信息泄露漏洞(MS16-019)</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32490</t>
-  </si>
-  <si>
-    <t>CVE-2016-0047</t>
-  </si>
-  <si>
-    <t>Microsoft Windows PDF Library缓冲区溢出漏洞(MS16-012)</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32489</t>
-  </si>
-  <si>
-    <t>CVE-2016-0058</t>
-  </si>
-  <si>
-    <t>Microsoft Windows Reader任意代码执行漏洞(MS16-012)</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32488</t>
-  </si>
-  <si>
-    <t>CVE-2016-0046</t>
-  </si>
-  <si>
-    <t>Microsoft Windows Journal内存破坏漏洞(MS16-013)</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32487</t>
-  </si>
-  <si>
-    <t>glibc getaddrinfo栈缓冲区溢出漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/32486</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>postgresql</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy\-mm\-dd\ h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="微軟正黑體"/>
+      <family val="2"/>
       <charset val="136"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1342,35 +1358,31 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="165" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="165" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="165" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="一般" xfId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -1658,23 +1670,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="17.375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="9.375"/>
-    <col customWidth="1" max="3" min="3" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="4" style="1" width="9"/>
+    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1807,29 +1815,36 @@
         <v>25</v>
       </c>
     </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" paperSize="9" verticalDpi="200"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="15.375"/>
-    <col customWidth="1" max="2" min="2" style="1" width="9"/>
-    <col customWidth="1" max="16384" min="3" style="1" width="9"/>
+    <col min="1" max="1" width="15.375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1877,25 +1892,35 @@
         <v>33</v>
       </c>
     </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" paperSize="9" verticalDpi="200"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -1921,159 +1946,159 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="6">
         <v>42411</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="4" t="n"/>
-      <c r="F2" s="4" t="n"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="9">
         <v>42417</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="9" t="n"/>
-      <c r="F3" s="9" t="n"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="6">
         <v>42417</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="4" t="n"/>
-      <c r="F4" s="4" t="n"/>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="6">
         <v>42416</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="4" t="n"/>
-      <c r="F5" s="4" t="n"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="6">
         <v>42416</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="4" t="n"/>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="4" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="9">
         <v>42416</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-      <c r="G7" s="9" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="13" t="n">
+      <c r="A8" s="9">
         <v>42416</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-      <c r="G8" s="9" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="6">
         <v>42415</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="4" t="n"/>
-      <c r="F9" s="4" t="n"/>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="12" t="n">
+      <c r="A10" s="8">
         <v>42415</v>
       </c>
       <c r="B10" t="s">
@@ -2096,26 +2121,26 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="6">
         <v>42415</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="12" t="n">
+      <c r="A12" s="8">
         <v>42415</v>
       </c>
       <c r="B12" t="s">
@@ -2138,106 +2163,106 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="6">
         <v>42416</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="4" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="6">
         <v>42416</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="6">
         <v>42415</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="4" t="n"/>
-      <c r="F15" s="4" t="n"/>
-      <c r="G15" s="4" t="s">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="6">
         <v>42415</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="4" t="n"/>
-      <c r="F16" s="4" t="n"/>
-      <c r="G16" s="4" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="6">
         <v>42415</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="4" t="n"/>
-      <c r="F17" s="4" t="n"/>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="12" t="n">
+      <c r="A18" s="8">
         <v>42417</v>
       </c>
       <c r="B18" t="s">
@@ -2260,7 +2285,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="12" t="n">
+      <c r="A19" s="8">
         <v>42415</v>
       </c>
       <c r="B19" t="s">
@@ -2283,7 +2308,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="12" t="n">
+      <c r="A20" s="8">
         <v>42411</v>
       </c>
       <c r="B20" t="s">
@@ -2306,58 +2331,58 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="10" t="n">
+      <c r="A21" s="6">
         <v>42411</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="4" t="n"/>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="4" t="n"/>
-      <c r="F21" s="4" t="n"/>
-      <c r="G21" s="4" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="11" t="n">
+      <c r="A22" s="7">
         <v>42411</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="6" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="6" t="n"/>
-      <c r="F22" s="6" t="n"/>
-      <c r="G22" s="6" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="10" t="n">
+      <c r="A23" s="6">
         <v>42411</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="4" t="n"/>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="4" t="n"/>
-      <c r="F23" s="4" t="n"/>
-      <c r="G23" s="4" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="12" t="n">
+      <c r="A24" s="8">
         <v>42411</v>
       </c>
       <c r="B24" t="s">
@@ -2380,7 +2405,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="12" t="n">
+      <c r="A25" s="8">
         <v>42411</v>
       </c>
       <c r="B25" t="s">
@@ -2403,28 +2428,28 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="10" t="n">
+      <c r="A26" s="6">
         <v>42411</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="F26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="12" t="n">
+      <c r="A27" s="8">
         <v>42411</v>
       </c>
       <c r="B27" t="s">
@@ -2447,24 +2472,24 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="10" t="n">
+      <c r="A28" s="6">
         <v>42411</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="4" t="n"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="4" t="n"/>
-      <c r="F28" s="4" t="n"/>
-      <c r="G28" s="4" t="s">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="12" t="n">
+      <c r="A29" s="8">
         <v>42411</v>
       </c>
       <c r="B29" t="s">
@@ -2487,7 +2512,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="12" t="n">
+      <c r="A30" s="8">
         <v>42411</v>
       </c>
       <c r="B30" t="s">
@@ -2510,7 +2535,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="12" t="n">
+      <c r="A31" s="8">
         <v>42411</v>
       </c>
       <c r="B31" t="s">
@@ -2533,26 +2558,26 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="11" t="n">
+      <c r="A32" s="7">
         <v>42411</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="6" t="n"/>
-      <c r="D32" s="6" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F32" s="6" t="n"/>
-      <c r="G32" s="6" t="s">
+      <c r="F32" s="4"/>
+      <c r="G32" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="12" t="n">
+      <c r="A33" s="8">
         <v>42411</v>
       </c>
       <c r="B33" t="s">
@@ -2575,7 +2600,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="12" t="n">
+      <c r="A34" s="8">
         <v>42411</v>
       </c>
       <c r="B34" t="s">
@@ -2598,7 +2623,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="12" t="n">
+      <c r="A35" s="8">
         <v>42411</v>
       </c>
       <c r="B35" t="s">
@@ -2621,7 +2646,7 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="12" t="n">
+      <c r="A36" s="8">
         <v>42411</v>
       </c>
       <c r="B36" t="s">
@@ -2644,7 +2669,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="12" t="n">
+      <c r="A37" s="8">
         <v>42411</v>
       </c>
       <c r="B37" t="s">
@@ -2667,7 +2692,7 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="12" t="n">
+      <c r="A38" s="8">
         <v>42411</v>
       </c>
       <c r="B38" t="s">
@@ -2690,304 +2715,304 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="10" t="n">
+      <c r="A39" s="6">
         <v>42417</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="4" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E39" s="4" t="n"/>
-      <c r="F39" s="4" t="n"/>
-      <c r="G39" s="4" t="s">
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="10" t="n">
+      <c r="A40" s="6">
         <v>42417</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E40" s="4" t="n"/>
-      <c r="F40" s="4" t="n"/>
-      <c r="G40" s="4" t="s">
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="11" t="n">
+      <c r="A41" s="7">
         <v>42417</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C41" s="6" t="n"/>
-      <c r="D41" s="6" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E41" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F41" s="6" t="n"/>
-      <c r="G41" s="6" t="s">
+      <c r="F41" s="4"/>
+      <c r="G41" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="11" t="n">
+      <c r="A42" s="7">
         <v>42417</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="6" t="n"/>
-      <c r="D42" s="6" t="s">
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="6" t="n"/>
-      <c r="G42" s="6" t="s">
+      <c r="F42" s="4"/>
+      <c r="G42" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="11" t="n">
+      <c r="A43" s="7">
         <v>42417</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C43" s="6" t="n"/>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="4"/>
+      <c r="D43" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F43" s="6" t="n"/>
-      <c r="G43" s="6" t="s">
+      <c r="F43" s="4"/>
+      <c r="G43" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="11" t="n">
+      <c r="A44" s="7">
         <v>42417</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C44" s="6" t="n"/>
-      <c r="D44" s="6" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F44" s="6" t="n"/>
-      <c r="G44" s="6" t="s">
+      <c r="F44" s="4"/>
+      <c r="G44" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="11" t="n">
+      <c r="A45" s="7">
         <v>42417</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C45" s="6" t="n"/>
-      <c r="D45" s="6" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E45" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F45" s="6" t="n"/>
-      <c r="G45" s="6" t="s">
+      <c r="F45" s="4"/>
+      <c r="G45" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="10" t="n">
+      <c r="A46" s="6">
         <v>42417</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C46" s="4" t="n"/>
-      <c r="D46" s="4" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G46" s="4" t="s">
+      <c r="F46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="10" t="n">
+      <c r="A47" s="6">
         <v>42416</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C47" s="4" t="n"/>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="4" t="s">
+      <c r="F47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="10" t="n">
+      <c r="A48" s="6">
         <v>42416</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C48" s="4" t="n"/>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G48" s="4" t="s">
+      <c r="F48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="10" t="n">
+      <c r="A49" s="6">
         <v>42416</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C49" s="4" t="n"/>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G49" s="4" t="s">
+      <c r="F49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="10" t="n">
+      <c r="A50" s="6">
         <v>42416</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C50" s="4" t="n"/>
-      <c r="D50" s="4" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G50" s="4" t="s">
+      <c r="F50" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="10" t="n">
+      <c r="A51" s="6">
         <v>42416</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C51" s="4" t="n"/>
-      <c r="D51" s="4" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G51" s="4" t="s">
+      <c r="F51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="10" t="n">
+      <c r="A52" s="6">
         <v>42416</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C52" s="4" t="n"/>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G52" s="4" t="s">
+      <c r="F52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="10" t="n">
+      <c r="A53" s="6">
         <v>42416</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C53" s="4" t="n"/>
-      <c r="D53" s="4" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G53" s="4" t="s">
+      <c r="F53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="12" t="n">
+      <c r="A54" s="8">
         <v>42416</v>
       </c>
       <c r="B54" t="s">
@@ -3010,45 +3035,45 @@
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="11" t="n">
+      <c r="A55" s="7">
         <v>42416</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C55" s="6" t="n"/>
-      <c r="D55" s="6" t="s">
+      <c r="C55" s="4"/>
+      <c r="D55" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F55" s="6" t="n"/>
-      <c r="G55" s="6" t="s">
+      <c r="F55" s="4"/>
+      <c r="G55" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="11" t="n">
+      <c r="A56" s="7">
         <v>42416</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C56" s="6" t="n"/>
-      <c r="D56" s="6" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="F56" s="6" t="n"/>
-      <c r="G56" s="6" t="s">
+      <c r="F56" s="4"/>
+      <c r="G56" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="12" t="n">
+      <c r="A57" s="8">
         <v>42416</v>
       </c>
       <c r="B57" t="s">
@@ -3071,7 +3096,7 @@
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="12" t="n">
+      <c r="A58" s="8">
         <v>42416</v>
       </c>
       <c r="B58" t="s">
@@ -3094,7 +3119,7 @@
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="12" t="n">
+      <c r="A59" s="8">
         <v>42416</v>
       </c>
       <c r="B59" t="s">
@@ -3117,49 +3142,49 @@
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="10" t="n">
+      <c r="A60" s="6">
         <v>42416</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="4" t="n"/>
-      <c r="D60" s="4" t="s">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" s="4" t="s">
+      <c r="F60" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="10" t="n">
+      <c r="A61" s="6">
         <v>42416</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C61" s="4" t="n"/>
-      <c r="D61" s="4" t="s">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G61" s="4" t="s">
+      <c r="F61" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="12" t="n">
+      <c r="A62" s="8">
         <v>42416</v>
       </c>
       <c r="B62" t="s">
@@ -3182,7 +3207,7 @@
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="12" t="n">
+      <c r="A63" s="8">
         <v>42416</v>
       </c>
       <c r="B63" t="s">
@@ -3205,70 +3230,70 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="10" t="n">
+      <c r="A64" s="6">
         <v>42416</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C64" s="4" t="n"/>
-      <c r="D64" s="4" t="s">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G64" s="4" t="s">
+      <c r="F64" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G64" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="10" t="n">
+      <c r="A65" s="6">
         <v>42416</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C65" s="4" t="n"/>
-      <c r="D65" s="4" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F65" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G65" s="4" t="s">
+      <c r="F65" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="10" t="n">
+      <c r="A66" s="6">
         <v>42416</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C66" s="4" t="n"/>
-      <c r="D66" s="4" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F66" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G66" s="4" t="s">
+      <c r="F66" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="12" t="n">
+      <c r="A67" s="8">
         <v>42416</v>
       </c>
       <c r="B67" t="s">
@@ -3291,7 +3316,7 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="12" t="n">
+      <c r="A68" s="8">
         <v>42416</v>
       </c>
       <c r="B68" t="s">
@@ -3314,83 +3339,83 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="11" t="n">
+      <c r="A69" s="7">
         <v>42415</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C69" s="6" t="n"/>
-      <c r="D69" s="6" t="s">
+      <c r="C69" s="4"/>
+      <c r="D69" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="E69" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F69" s="6" t="n"/>
-      <c r="G69" s="6" t="s">
+      <c r="F69" s="4"/>
+      <c r="G69" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="11" t="n">
+      <c r="A70" s="7">
         <v>42415</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C70" s="6" t="n"/>
-      <c r="D70" s="6" t="s">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="E70" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="F70" s="6" t="n"/>
-      <c r="G70" s="6" t="s">
+      <c r="F70" s="4"/>
+      <c r="G70" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="11" t="n">
+      <c r="A71" s="7">
         <v>42415</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C71" s="6" t="n"/>
-      <c r="D71" s="6" t="s">
+      <c r="C71" s="4"/>
+      <c r="D71" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="F71" s="6" t="n"/>
-      <c r="G71" s="6" t="s">
+      <c r="F71" s="4"/>
+      <c r="G71" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="11" t="n">
+      <c r="A72" s="7">
         <v>42415</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C72" s="6" t="n"/>
-      <c r="D72" s="6" t="s">
+      <c r="C72" s="4"/>
+      <c r="D72" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="F72" s="6" t="n"/>
-      <c r="G72" s="6" t="s">
+      <c r="F72" s="4"/>
+      <c r="G72" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="A73" s="12" t="n">
+      <c r="A73" s="8">
         <v>42415</v>
       </c>
       <c r="B73" t="s">
@@ -3413,7 +3438,7 @@
       </c>
     </row>
     <row r="74" spans="1:7">
-      <c r="A74" s="12" t="n">
+      <c r="A74" s="8">
         <v>42415</v>
       </c>
       <c r="B74" t="s">
@@ -3436,42 +3461,39 @@
       </c>
     </row>
     <row r="75" spans="1:7">
-      <c r="A75" s="11" t="n">
+      <c r="A75" s="7">
         <v>42415</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C75" s="6" t="n"/>
-      <c r="D75" s="6" t="s">
+      <c r="C75" s="4"/>
+      <c r="D75" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="E75" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F75" s="6" t="n"/>
-      <c r="G75" s="6" t="s">
+      <c r="F75" s="4"/>
+      <c r="G75" s="4" t="s">
         <v>127</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -3497,380 +3519,380 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="10" t="n">
+      <c r="A2" s="6">
         <v>42423</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E2" s="4" t="s"/>
-      <c r="F2" s="4" t="s"/>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="10" t="n">
+      <c r="A3" s="6">
         <v>42422</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="4" t="s"/>
-      <c r="F3" s="4" t="s"/>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="6">
         <v>42422</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="6">
         <v>42422</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E5" s="4" t="s"/>
-      <c r="F5" s="4" t="s"/>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="6">
         <v>42420</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="E6" s="4" t="s"/>
-      <c r="F6" s="4" t="s"/>
-      <c r="G6" s="4" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="6">
         <v>42419</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="4" t="s"/>
-      <c r="F7" s="4" t="s"/>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="6">
         <v>42419</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="E8" s="4" t="s"/>
-      <c r="F8" s="4" t="s"/>
-      <c r="G8" s="4" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="6">
         <v>42419</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E9" s="4" t="s"/>
-      <c r="F9" s="4" t="s"/>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="6">
         <v>42418</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E10" s="4" t="s"/>
-      <c r="F10" s="4" t="s"/>
-      <c r="G10" s="4" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="6">
         <v>42418</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="E11" s="4" t="s"/>
-      <c r="F11" s="4" t="s"/>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="6">
         <v>42422</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="E12" s="4" t="s"/>
-      <c r="F12" s="4" t="s"/>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="6">
         <v>42423</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="F13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="9">
         <v>42422</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="E14" s="9" t="s"/>
-      <c r="F14" s="9" t="s"/>
-      <c r="G14" s="9" t="s">
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="9">
         <v>42422</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="E15" s="9" t="s"/>
-      <c r="F15" s="9" t="s"/>
-      <c r="G15" s="9" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="9">
         <v>42422</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="E16" s="9" t="s"/>
-      <c r="F16" s="9" t="s"/>
-      <c r="G16" s="9" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="6">
         <v>42419</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E17" s="4" t="s"/>
-      <c r="F17" s="4" t="s"/>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="6">
         <v>42419</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="E18" s="4" t="s"/>
-      <c r="F18" s="4" t="s"/>
-      <c r="G18" s="4" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="10" t="n">
+      <c r="A19" s="6">
         <v>42419</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="E19" s="4" t="s"/>
-      <c r="F19" s="4" t="s"/>
-      <c r="G19" s="4" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="6">
         <v>42419</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="F20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="12" t="n">
+      <c r="A21" s="8">
         <v>42419</v>
       </c>
       <c r="B21" t="s">
@@ -3893,7 +3915,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="12" t="n">
+      <c r="A22" s="8">
         <v>42424</v>
       </c>
       <c r="B22" t="s">
@@ -3916,7 +3938,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="12" t="n">
+      <c r="A23" s="8">
         <v>42423</v>
       </c>
       <c r="B23" t="s">
@@ -3939,131 +3961,131 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="11" t="n">
+      <c r="A24" s="7">
         <v>42418</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C24" s="6" t="s"/>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="6" t="s"/>
-      <c r="G24" s="6" t="s">
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="10" t="n">
+      <c r="A25" s="6">
         <v>42418</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="C25" s="4" t="s"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="10" t="n">
+      <c r="A26" s="6">
         <v>42424</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="C26" s="4" t="s"/>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="F26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="10" t="n">
+      <c r="A27" s="6">
         <v>42424</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C27" s="4" t="s"/>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="4" t="s">
+      <c r="F27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="10" t="n">
+      <c r="A28" s="6">
         <v>42424</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C28" s="4" t="s"/>
-      <c r="D28" s="4" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="4" t="s">
+      <c r="F28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="10" t="n">
+      <c r="A29" s="6">
         <v>42424</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="C29" s="4" t="s"/>
-      <c r="D29" s="4" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="4" t="s">
+      <c r="F29" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="12" t="n">
+      <c r="A30" s="8">
         <v>42423</v>
       </c>
       <c r="B30" t="s">
@@ -4086,26 +4108,26 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="11" t="n">
+      <c r="A31" s="7">
         <v>42423</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="C31" s="6" t="s"/>
-      <c r="D31" s="6" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="F31" s="6" t="s"/>
-      <c r="G31" s="6" t="s">
+      <c r="F31" s="4"/>
+      <c r="G31" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="12" t="n">
+      <c r="A32" s="8">
         <v>42423</v>
       </c>
       <c r="B32" t="s">
@@ -4128,104 +4150,104 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="11" t="n">
+      <c r="A33" s="7">
         <v>42423</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="C33" s="6" t="s"/>
-      <c r="D33" s="6" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="F33" s="6" t="s"/>
-      <c r="G33" s="6" t="s">
+      <c r="F33" s="4"/>
+      <c r="G33" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="11" t="n">
+      <c r="A34" s="7">
         <v>42423</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C34" s="6" t="s"/>
-      <c r="D34" s="6" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="F34" s="6" t="s"/>
-      <c r="G34" s="6" t="s">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="11" t="n">
+      <c r="A35" s="7">
         <v>42423</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C35" s="6" t="s"/>
-      <c r="D35" s="6" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="F35" s="6" t="s"/>
-      <c r="G35" s="6" t="s">
+      <c r="F35" s="4"/>
+      <c r="G35" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="11" t="n">
+      <c r="A36" s="7">
         <v>42423</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="C36" s="6" t="s"/>
-      <c r="D36" s="6" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="F36" s="6" t="s"/>
-      <c r="G36" s="6" t="s">
+      <c r="F36" s="4"/>
+      <c r="G36" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="6">
         <v>42422</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C37" s="4" t="s"/>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="4" t="s">
+      <c r="F37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="12" t="n">
+      <c r="A38" s="8">
         <v>42422</v>
       </c>
       <c r="B38" t="s">
@@ -4248,7 +4270,7 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="12" t="n">
+      <c r="A39" s="8">
         <v>42422</v>
       </c>
       <c r="B39" t="s">
@@ -4271,7 +4293,7 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="12" t="n">
+      <c r="A40" s="8">
         <v>42422</v>
       </c>
       <c r="B40" t="s">
@@ -4294,7 +4316,7 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="12" t="n">
+      <c r="A41" s="8">
         <v>42422</v>
       </c>
       <c r="B41" t="s">
@@ -4317,7 +4339,7 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="12" t="n">
+      <c r="A42" s="8">
         <v>42422</v>
       </c>
       <c r="B42" t="s">
@@ -4340,7 +4362,7 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="12" t="n">
+      <c r="A43" s="8">
         <v>42422</v>
       </c>
       <c r="B43" t="s">
@@ -4363,26 +4385,26 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="11" t="n">
+      <c r="A44" s="7">
         <v>42422</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C44" s="6" t="s"/>
-      <c r="D44" s="6" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="F44" s="6" t="s"/>
-      <c r="G44" s="6" t="s">
+      <c r="F44" s="4"/>
+      <c r="G44" s="4" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="12" t="n">
+      <c r="A45" s="8">
         <v>42422</v>
       </c>
       <c r="B45" t="s">
@@ -4405,7 +4427,7 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="12" t="n">
+      <c r="A46" s="8">
         <v>42422</v>
       </c>
       <c r="B46" t="s">
@@ -4428,49 +4450,49 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="10" t="n">
+      <c r="A47" s="6">
         <v>42419</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="C47" s="4" t="s"/>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="4" t="s">
+      <c r="F47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="10" t="n">
+      <c r="A48" s="6">
         <v>42419</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="C48" s="4" t="s"/>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G48" s="4" t="s">
+      <c r="F48" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="12" t="n">
+      <c r="A49" s="8">
         <v>42419</v>
       </c>
       <c r="B49" t="s">
@@ -4493,7 +4515,7 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="12" t="n">
+      <c r="A50" s="8">
         <v>42419</v>
       </c>
       <c r="B50" t="s">
@@ -4516,284 +4538,285 @@
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="10" t="n">
+      <c r="A51" s="6">
         <v>42419</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="C51" s="4" t="s"/>
-      <c r="D51" s="4" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G51" s="4" t="s">
+      <c r="F51" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="10" t="n">
+      <c r="A52" s="6">
         <v>42419</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="C52" s="4" t="s"/>
-      <c r="D52" s="4" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G52" s="4" t="s">
+      <c r="F52" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="10" t="n">
+      <c r="A53" s="6">
         <v>42419</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="C53" s="4" t="s"/>
-      <c r="D53" s="4" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G53" s="4" t="s">
+      <c r="F53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="10" t="n">
+      <c r="A54" s="6">
         <v>42419</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C54" s="4" t="s"/>
-      <c r="D54" s="4" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G54" s="4" t="s">
+      <c r="F54" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="11" t="n">
+      <c r="A55" s="7">
         <v>42418</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="C55" s="6" t="s"/>
-      <c r="D55" s="6" t="s">
+      <c r="C55" s="4"/>
+      <c r="D55" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="E55" s="6" t="s">
+      <c r="E55" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="F55" s="6" t="s"/>
-      <c r="G55" s="6" t="s">
+      <c r="F55" s="4"/>
+      <c r="G55" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="11" t="n">
+      <c r="A56" s="7">
         <v>42418</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C56" s="6" t="s"/>
-      <c r="D56" s="6" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="F56" s="6" t="s"/>
-      <c r="G56" s="6" t="s">
+      <c r="F56" s="4"/>
+      <c r="G56" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="10" t="n">
+      <c r="A57" s="6">
         <v>42418</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="C57" s="4" t="s"/>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="F57" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="6">
+        <v>42418</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G57" s="4" t="s">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="10" t="n">
+    <row r="59" spans="1:7">
+      <c r="A59" s="7">
         <v>42418</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="C58" s="4" t="s"/>
-      <c r="D58" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="E58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="11" t="n">
+      <c r="C59" s="4"/>
+      <c r="D59" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="7">
         <v>42418</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="C59" s="6" t="s"/>
-      <c r="D59" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="E59" s="6" t="s">
+      <c r="B60" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="F59" s="6" t="s"/>
-      <c r="G59" s="6" t="s">
+      <c r="C60" s="4"/>
+      <c r="D60" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="11" t="n">
+    <row r="61" spans="1:7">
+      <c r="A61" s="7">
         <v>42418</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>405</v>
-      </c>
-      <c r="C60" s="6" t="s"/>
-      <c r="D60" s="6" t="s">
-        <v>406</v>
-      </c>
-      <c r="E60" s="6" t="s">
+      <c r="B61" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="F60" s="6" t="s"/>
-      <c r="G60" s="6" t="s">
+      <c r="C61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="11" t="n">
+    <row r="62" spans="1:7">
+      <c r="A62" s="7">
         <v>42418</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="C61" s="6" t="s"/>
-      <c r="D61" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="E61" s="6" t="s">
+      <c r="B62" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="F61" s="6" t="s"/>
-      <c r="G61" s="6" t="s">
+      <c r="C62" s="4"/>
+      <c r="D62" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="11" t="n">
+    <row r="63" spans="1:7">
+      <c r="A63" s="7">
         <v>42418</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>411</v>
-      </c>
-      <c r="C62" s="6" t="s"/>
-      <c r="D62" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="E62" s="6" t="s">
+      <c r="B63" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="F62" s="6" t="s"/>
-      <c r="G62" s="6" t="s">
+      <c r="C63" s="4"/>
+      <c r="D63" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="11" t="n">
+    <row r="64" spans="1:7">
+      <c r="A64" s="7">
         <v>42418</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="C63" s="6" t="s"/>
-      <c r="D63" s="6" t="s">
+      <c r="B64" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F63" s="6" t="s"/>
-      <c r="G63" s="6" t="s">
+      <c r="C64" s="4"/>
+      <c r="D64" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="11" t="n">
-        <v>42418</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="C64" s="6" t="s"/>
-      <c r="D64" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F64" s="6" t="s"/>
-      <c r="G64" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>